<commit_message>
eddy ni 1986-1987 (update)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
+++ b/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14340" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="192">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -556,16 +556,10 @@
     <t>Van der Helstraeten Jean-Jacques</t>
   </si>
   <si>
-    <t>Roque 5 degradeert; Carnières blijft in 3de afdeling</t>
-  </si>
-  <si>
     <t>berekening matchpunten  1 of 0,5 of 0</t>
   </si>
   <si>
     <t>promoveert</t>
-  </si>
-  <si>
-    <t>beslissing NTL:  Anderlecht 4 - Tibechecs  3-0</t>
   </si>
   <si>
     <t>Dworp 2 promoveert dankzij vacante plaats</t>
@@ -589,12 +583,6 @@
     <t xml:space="preserve">Willebroek maakte in R7 waarschijnlijk een opstelllingsfout tegen Dworp 3 </t>
   </si>
   <si>
-    <t>einduitslag: Willebroek kreeg 13,5 en Dworp 8,5.</t>
-  </si>
-  <si>
-    <t>ik weet natuurlijk niet op welk bord. Kan je dat computergestuurd verwoorden?</t>
-  </si>
-  <si>
     <t>Verbruggen Jan</t>
   </si>
   <si>
@@ -605,6 +593,15 @@
   </si>
   <si>
     <t>Pax Walter</t>
+  </si>
+  <si>
+    <t>5G beslissing NTL:  Anderlecht 4 - Tibechecs  3-0</t>
+  </si>
+  <si>
+    <t>5K   einduitslag: Willebroek kreeg 13,5 en Dworp 8,5.</t>
+  </si>
+  <si>
+    <t>3B Roque 5 degradeert; Carnières blijft in 3de afdeling</t>
   </si>
 </sst>
 </file>
@@ -702,7 +699,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,13 +756,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1224,7 +1215,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1431,13 +1422,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1739,11 +1724,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1753,13 +1736,13 @@
     <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:13">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:10">
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
@@ -1767,13 +1750,13 @@
         <v>1986</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="71"/>
       <c r="F3" s="71"/>
       <c r="G3" s="71"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="23" t="s">
         <v>38</v>
       </c>
@@ -1781,43 +1764,23 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:10">
       <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="70" t="s">
-        <v>179</v>
-      </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="J6" s="71" t="s">
-        <v>180</v>
-      </c>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="24" t="s">
         <v>3</v>
       </c>
@@ -1825,47 +1788,63 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="30"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="D9" s="80" t="s">
-        <v>187</v>
-      </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="D10" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="D11" s="70" t="s">
-        <v>188</v>
-      </c>
+    <row r="11" spans="1:10">
+      <c r="C11" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="70"/>
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
       <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="C12" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="C14" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1985,7 +1964,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -3789,7 +3768,7 @@
   <dimension ref="A1:AQ280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4197,7 +4176,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" s="41">
         <v>1</v>
@@ -5913,7 +5892,7 @@
         <v>6</v>
       </c>
       <c r="R19" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S19" s="54">
         <f>IF(C19="","",IF(C19&gt;D18,1,IF(C19=D18,0.5,0)))</f>
@@ -6438,7 +6417,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="41">
         <v>1</v>
@@ -7731,7 +7710,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C34" s="41">
         <v>2</v>
@@ -7883,11 +7862,11 @@
       <c r="E35" s="41">
         <v>3</v>
       </c>
-      <c r="F35" s="68" t="s">
+      <c r="F35" s="40" t="s">
         <v>37</v>
       </c>
       <c r="G35" s="68">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="H35" s="41">
         <v>2</v>
@@ -7900,9 +7879,9 @@
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
       <c r="N35" s="41"/>
-      <c r="O35" s="78">
+      <c r="O35" s="42">
         <f t="shared" si="31"/>
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="P35" s="43">
         <f t="shared" si="33"/>
@@ -7912,9 +7891,7 @@
         <f t="shared" si="32"/>
         <v>6</v>
       </c>
-      <c r="R35" s="79">
-        <v>13.5</v>
-      </c>
+      <c r="R35" s="52"/>
       <c r="S35" s="54">
         <f>IF(C35="","",IF(C35&gt;$F32,1,IF(C35=$F32,0.5,0)))</f>
         <v>0.5</v>
@@ -8027,9 +8004,9 @@
         <v>1</v>
       </c>
       <c r="F36" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="G36" s="68" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="G36" s="40" t="s">
         <v>37</v>
       </c>
       <c r="H36" s="41">
@@ -8043,9 +8020,9 @@
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
       <c r="N36" s="41"/>
-      <c r="O36" s="78">
+      <c r="O36" s="42">
         <f t="shared" si="31"/>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="P36" s="43">
         <f t="shared" si="33"/>
@@ -8055,9 +8032,7 @@
         <f t="shared" si="32"/>
         <v>6</v>
       </c>
-      <c r="R36" s="79">
-        <v>8.5</v>
-      </c>
+      <c r="R36" s="52"/>
       <c r="S36" s="54">
         <f>IF(C36="","",IF(C36&gt;$G32,1,IF(C36=$G32,0.5,0)))</f>
         <v>0</v>
@@ -8158,7 +8133,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C37" s="41">
         <v>0</v>
@@ -15086,7 +15061,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -15691,7 +15666,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -15892,7 +15867,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -16248,7 +16223,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -18518,7 +18493,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19048,7 +19023,7 @@
         <v>22373</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -19078,17 +19053,17 @@
         <v>7331</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="19">
         <v>27715</v>
@@ -19108,17 +19083,17 @@
         <v>6998</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="19">
         <v>97453</v>
@@ -19138,17 +19113,17 @@
         <v>22624</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="19">
         <v>33910</v>
@@ -19169,13 +19144,13 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="13">
         <v>0.5</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="13">
-        <v>3.5</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="16">

</xml_diff>

<commit_message>
eddy ni 1986-1987 (update 3)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
+++ b/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870"/>
+    <workbookView xWindow="14340" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="204">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>3B Roque 5 degradeert na een degradatieduel tegen Soignies 1 (bron Le Pion F, nummer 20, april 87)</t>
+  </si>
+  <si>
+    <t>17,5?</t>
+  </si>
+  <si>
+    <t>5?</t>
   </si>
 </sst>
 </file>
@@ -1535,14 +1541,14 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="9" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1848,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1999,8 +2005,8 @@
       <c r="G17" s="63"/>
       <c r="H17" s="63"/>
       <c r="I17" s="63"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
       <c r="L17" s="63"/>
       <c r="M17" s="63"/>
     </row>
@@ -3919,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD280"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6639,7 +6645,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
-      <c r="O19" s="95">
+      <c r="O19" s="94">
         <f t="shared" si="6"/>
         <v>16.5</v>
       </c>
@@ -6651,8 +6657,8 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="R19" s="94">
-        <v>17.5</v>
+      <c r="R19" s="97" t="s">
+        <v>202</v>
       </c>
       <c r="S19" s="47">
         <f>IF(C19="","",IF(C19&gt;D18,1,IF(C19=D18,0.5,0)))</f>
@@ -6912,7 +6918,7 @@
         <f>H20+E23</f>
         <v>4</v>
       </c>
-      <c r="AL20" s="97">
+      <c r="AL20" s="96">
         <f>I20+E24</f>
         <v>3</v>
       </c>
@@ -7581,7 +7587,7 @@
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
-      <c r="O24" s="95">
+      <c r="O24" s="94">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -7593,8 +7599,8 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="R24" s="94">
-        <v>5</v>
+      <c r="R24" s="97" t="s">
+        <v>203</v>
       </c>
       <c r="S24" s="47">
         <f>IF(C24="","",IF(C24&gt;$I18,1,IF(C24=$I18,0.5,0)))</f>
@@ -7651,7 +7657,7 @@
         <f>D24+I19</f>
         <v>4</v>
       </c>
-      <c r="AH24" s="97">
+      <c r="AH24" s="96">
         <f>E24+I20</f>
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
eddy ni 1986-1987 (update 5)
</commit_message>
<xml_diff>
--- a/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
+++ b/_data/ni/ni8687/individueel_eindstand_dworp_123_8687.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="220">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -675,6 +675,18 @@
   <si>
     <t>5?</t>
   </si>
+  <si>
+    <t>dat ik na iedere ronde bijwerkte. Dat rooster deed dus ook dienst als kladwerk voor mijn nota's (volgens eindrangschikking) waar ik tegenwoordig steevast uit put.</t>
+  </si>
+  <si>
+    <t>eddy op 18 aug '17:  toen ik jouw kopieën uit le pion f klasseerde bij de andere officiële archiefstukken, vond ik het rooster (volgens lotingsnummers)</t>
+  </si>
+  <si>
+    <t>Zo is het tenminste duidelijk dat Tibechecs geen fout maakte.</t>
+  </si>
+  <si>
+    <t>In dat bewuste kladwerk is de uitslag 4-0 met rode bic aangepast naar 3-1 wegens opstellingsfout.</t>
+  </si>
 </sst>
 </file>
 
@@ -780,7 +792,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,6 +886,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,7 +1352,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1587,6 +1605,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19404,10 +19424,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19832,7 +19852,7 @@
       <c r="V16" s="63"/>
       <c r="W16" s="63"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:27">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -19874,7 +19894,7 @@
       <c r="V17" s="63"/>
       <c r="W17" s="63"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" thickBot="1">
+    <row r="18" spans="1:27" ht="15.75" thickBot="1">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -19916,7 +19936,7 @@
       <c r="V18" s="63"/>
       <c r="W18" s="63"/>
     </row>
-    <row r="19" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
+    <row r="19" spans="1:27" ht="16.5" thickTop="1" thickBot="1">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="16">
@@ -19954,7 +19974,7 @@
       <c r="V19" s="63"/>
       <c r="W19" s="63"/>
     </row>
-    <row r="20" spans="1:23" ht="19.5" thickBot="1">
+    <row r="20" spans="1:27" ht="19.5" thickBot="1">
       <c r="A20" s="17" t="s">
         <v>16</v>
       </c>
@@ -19969,7 +19989,7 @@
       <c r="R20" s="62"/>
       <c r="S20" s="62"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:27">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>11</v>
@@ -19997,7 +20017,7 @@
       <c r="R21" s="62"/>
       <c r="S21" s="62"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:27">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -20037,7 +20057,7 @@
       <c r="R22" s="62"/>
       <c r="S22" s="62"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:27">
       <c r="A23" s="5">
         <v>1</v>
       </c>
@@ -20065,7 +20085,7 @@
       <c r="R23" s="62"/>
       <c r="S23" s="62"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:27">
       <c r="A24" s="5">
         <v>2</v>
       </c>
@@ -20093,7 +20113,7 @@
       <c r="R24" s="62"/>
       <c r="S24" s="62"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:27">
       <c r="A25" s="5">
         <v>3</v>
       </c>
@@ -20110,8 +20130,26 @@
       <c r="H25" s="19"/>
       <c r="I25" s="14"/>
       <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="1:23" ht="15.75" thickBot="1">
+      <c r="L25" s="98" t="s">
+        <v>217</v>
+      </c>
+      <c r="M25" s="99"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="99"/>
+      <c r="P25" s="99"/>
+      <c r="Q25" s="99"/>
+      <c r="R25" s="99"/>
+      <c r="S25" s="99"/>
+      <c r="T25" s="99"/>
+      <c r="U25" s="99"/>
+      <c r="V25" s="99"/>
+      <c r="W25" s="99"/>
+      <c r="X25" s="99"/>
+      <c r="Y25" s="99"/>
+      <c r="Z25" s="99"/>
+      <c r="AA25" s="99"/>
+    </row>
+    <row r="26" spans="1:27" ht="15.75" thickBot="1">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -20128,8 +20166,26 @@
       <c r="H26" s="19"/>
       <c r="I26" s="14"/>
       <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:23" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L26" s="99" t="s">
+        <v>216</v>
+      </c>
+      <c r="M26" s="99"/>
+      <c r="N26" s="99"/>
+      <c r="O26" s="99"/>
+      <c r="P26" s="99"/>
+      <c r="Q26" s="99"/>
+      <c r="R26" s="99"/>
+      <c r="S26" s="99"/>
+      <c r="T26" s="99"/>
+      <c r="U26" s="99"/>
+      <c r="V26" s="99"/>
+      <c r="W26" s="99"/>
+      <c r="X26" s="99"/>
+      <c r="Y26" s="99"/>
+      <c r="Z26" s="99"/>
+      <c r="AA26" s="99"/>
+    </row>
+    <row r="27" spans="1:27" ht="16.5" thickTop="1" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="16" t="str">
@@ -20148,13 +20204,49 @@
         <v/>
       </c>
       <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:23" ht="19.5" thickBot="1">
+      <c r="L27" s="99" t="s">
+        <v>219</v>
+      </c>
+      <c r="M27" s="99"/>
+      <c r="N27" s="99"/>
+      <c r="O27" s="99"/>
+      <c r="P27" s="99"/>
+      <c r="Q27" s="99"/>
+      <c r="R27" s="99"/>
+      <c r="S27" s="99"/>
+      <c r="T27" s="99"/>
+      <c r="U27" s="99"/>
+      <c r="V27" s="99"/>
+      <c r="W27" s="99"/>
+      <c r="X27" s="99"/>
+      <c r="Y27" s="99"/>
+      <c r="Z27" s="99"/>
+      <c r="AA27" s="99"/>
+    </row>
+    <row r="28" spans="1:27" ht="19.5" thickBot="1">
       <c r="A28" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="L28" s="99" t="s">
+        <v>218</v>
+      </c>
+      <c r="M28" s="99"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
+      <c r="T28" s="99"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="99"/>
+      <c r="W28" s="99"/>
+      <c r="X28" s="99"/>
+      <c r="Y28" s="99"/>
+      <c r="Z28" s="99"/>
+      <c r="AA28" s="99"/>
+    </row>
+    <row r="29" spans="1:27">
       <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>11</v>
@@ -20170,7 +20262,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:27">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -20200,7 +20292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:27">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -20216,7 +20308,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:27">
       <c r="A32" s="5">
         <v>2</v>
       </c>

</xml_diff>